<commit_message>
make tables, plot and analysis
</commit_message>
<xml_diff>
--- a/age_group.xlsx
+++ b/age_group.xlsx
@@ -365,22 +365,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>anaemia_count</t>
+          <t>FALSE_count</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>anaemia_percent</t>
+          <t>FALSE_percent</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>no anaemia_count</t>
+          <t>TRUE_count</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>no anaemia_percent</t>
+          <t>TRUE_percent</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -401,16 +401,16 @@
         </is>
       </c>
       <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>16.66666666666666</v>
+      </c>
+      <c r="D2">
         <v>18</v>
       </c>
-      <c r="C2">
-        <v>24.65753424657534</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
       <c r="E2">
-        <v>15.78947368421053</v>
+        <v>24.32432432432433</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -426,16 +426,16 @@
         </is>
       </c>
       <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>16.66666666666666</v>
+      </c>
+      <c r="D3">
         <v>18</v>
       </c>
-      <c r="C3">
-        <v>24.65753424657534</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
       <c r="E3">
-        <v>15.78947368421053</v>
+        <v>24.32432432432433</v>
       </c>
       <c r="F3">
         <v>7</v>
@@ -451,16 +451,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>23.28767123287671</v>
+        <v>38.88888888888889</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E4">
-        <v>42.10526315789473</v>
+        <v>24.32432432432433</v>
       </c>
       <c r="F4">
         <v>14</v>
@@ -476,16 +476,16 @@
         </is>
       </c>
       <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>22.22222222222222</v>
+      </c>
+      <c r="D5">
         <v>8</v>
       </c>
-      <c r="C5">
-        <v>10.95890410958904</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
       <c r="E5">
-        <v>21.05263157894737</v>
+        <v>10.81081081081081</v>
       </c>
       <c r="F5">
         <v>9</v>
@@ -497,45 +497,45 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>35 to 39, years</t>
+          <t>40 to 44 years</t>
         </is>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>10.95890410958904</v>
+        <v>5.555555555555555</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>5.405405405405405</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>2.564102564102564</v>
+        <v>7.692307692307693</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>40 to 44 years</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>5.47945205479452</v>
+          <t>35 to 39 years</t>
+        </is>
       </c>
       <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>10.81081081081081</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>5.263157894736842</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
       <c r="G7">
-        <v>7.692307692307693</v>
+        <v>2.564102564102564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>